<commit_message>
made the impact factor table in excel
</commit_message>
<xml_diff>
--- a/paper/Impact Factors.xlsx
+++ b/paper/Impact Factors.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/addiew/Documents/GitHub/Outliers/paper/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186AE8BC-5E60-DE41-A9E9-3C459535AED4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="480" yWindow="700" windowWidth="25600" windowHeight="15480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table from Outline" sheetId="2" r:id="rId2"/>
+    <sheet name="2012 and 2017 Impact Factors" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$114</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
   <si>
     <t>Subject</t>
   </si>
@@ -495,13 +501,181 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Impact Factor 2012</t>
+  </si>
+  <si>
+    <t>Impact Factor 2017</t>
+  </si>
+  <si>
+    <t>Number of Experiments 2012</t>
+  </si>
+  <si>
+    <t>Number of Experiments 2017</t>
+  </si>
+  <si>
+    <t>Proportion Change</t>
+  </si>
+  <si>
+    <t>(5 year 4.95)</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology: Learning, Memory, and Cognition</t>
+  </si>
+  <si>
+    <t>(5 year 2.96)</t>
+  </si>
+  <si>
+    <t>Journal of Counseling Psychology</t>
+  </si>
+  <si>
+    <t>(5 year 4.09)</t>
+  </si>
+  <si>
+    <t>(5 year 3.32)</t>
+  </si>
+  <si>
+    <t>Journal of Youth and Adolescence</t>
+  </si>
+  <si>
+    <t>(5 year 3.96)</t>
+  </si>
+  <si>
+    <t>(5 year 5.24)</t>
+  </si>
+  <si>
+    <t>(5 year 4.08)</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>(5 year 4.46)</t>
+  </si>
+  <si>
+    <t>Psychology, Public Policy, and Law</t>
+  </si>
+  <si>
+    <t>(5 year 2.24)</t>
+  </si>
+  <si>
+    <t>(5 year 2.92)</t>
+  </si>
+  <si>
+    <t>Industrial Organizational</t>
+  </si>
+  <si>
+    <t>Organizational Behavior and Human Decision Process</t>
+  </si>
+  <si>
+    <t>Neurological/ Physiological</t>
+  </si>
+  <si>
+    <t>(5 year 3.73)</t>
+  </si>
+  <si>
+    <t>Cognitive, Affective, and Behavioral Neuroscience</t>
+  </si>
+  <si>
+    <t>(5 year 3.5)</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>(5 year 7.30)</t>
+  </si>
+  <si>
+    <t>(5 year 2.97)</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Journal of Sport &amp; Exercise Psychology</t>
+  </si>
+  <si>
+    <t>Human Kinetics</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Psychonomic Bulletin &amp; Review</t>
+  </si>
+  <si>
+    <t>(5 year 3.49)</t>
+  </si>
+  <si>
+    <t>Psychonomic Science</t>
+  </si>
+  <si>
+    <t>3.31 (5 year 3.92)</t>
+  </si>
+  <si>
+    <t>3.72 (5 year 4.95)</t>
+  </si>
+  <si>
+    <t>2.67 (5 year 2.96)</t>
+  </si>
+  <si>
+    <t>2.52 (5 year 4.09)</t>
+  </si>
+  <si>
+    <t>2.6 (5 year 3.32)</t>
+  </si>
+  <si>
+    <t>3.28 (5 year 3.96)</t>
+  </si>
+  <si>
+    <t>3.46(5 year 5.24)</t>
+  </si>
+  <si>
+    <t>2.88 (5 year 4.08)</t>
+  </si>
+  <si>
+    <t>3.49 (5 year 4.46)</t>
+  </si>
+  <si>
+    <t>1.92 (5 year 2.24)</t>
+  </si>
+  <si>
+    <t>2.82 (5 year 2.92)</t>
+  </si>
+  <si>
+    <t>2.45 (5 year 3.96)</t>
+  </si>
+  <si>
+    <t>3.29 (5 year 3.73)</t>
+  </si>
+  <si>
+    <t>3.26 (5 year 3.5)</t>
+  </si>
+  <si>
+    <t>5.02 (5 year 7.30)</t>
+  </si>
+  <si>
+    <t>2.16 (5 year 2.97)</t>
+  </si>
+  <si>
+    <t>2.92 (5 year 3.49)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +713,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -548,12 +747,117 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -619,7 +923,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -630,6 +934,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -698,6 +1050,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -989,14 +1344,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1005,7 +1360,7 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -1039,7 +1394,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1056,7 +1411,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -1073,7 +1428,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -1090,7 +1445,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -1107,7 +1462,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -1124,7 +1479,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1141,7 +1496,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1158,7 +1513,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1175,7 +1530,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1189,7 +1544,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1203,7 +1558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>90</v>
       </c>
@@ -1217,7 +1572,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1234,7 +1589,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1251,7 +1606,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -1265,7 +1620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1279,7 +1634,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>77</v>
       </c>
@@ -1293,7 +1648,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -1307,7 +1662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -1321,7 +1676,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>121</v>
       </c>
@@ -1338,7 +1693,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -1355,7 +1710,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -1372,7 +1727,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -1389,7 +1744,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>125</v>
       </c>
@@ -1403,7 +1758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>121</v>
       </c>
@@ -1417,7 +1772,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1434,7 +1789,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1451,7 +1806,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1465,7 +1820,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>47</v>
       </c>
@@ -1479,7 +1834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>47</v>
       </c>
@@ -1493,7 +1848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -1507,7 +1862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
@@ -1521,7 +1876,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -1535,7 +1890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1552,7 +1907,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1569,7 +1924,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1583,7 +1938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1597,7 +1952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1611,7 +1966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>138</v>
       </c>
@@ -1628,7 +1983,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>138</v>
       </c>
@@ -1645,7 +2000,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>138</v>
       </c>
@@ -1659,7 +2014,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
@@ -1676,7 +2031,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -1693,7 +2048,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>130</v>
       </c>
@@ -1704,7 +2059,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
@@ -1715,7 +2070,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>114</v>
       </c>
@@ -1729,7 +2084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>114</v>
       </c>
@@ -1743,7 +2098,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>114</v>
       </c>
@@ -1757,7 +2112,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>114</v>
       </c>
@@ -1771,7 +2126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -1788,7 +2143,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>152</v>
       </c>
@@ -1805,7 +2160,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>105</v>
       </c>
@@ -1822,7 +2177,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>105</v>
       </c>
@@ -1839,7 +2194,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>105</v>
       </c>
@@ -1853,7 +2208,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>105</v>
       </c>
@@ -1864,7 +2219,7 @@
         <v>5.6079999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>105</v>
       </c>
@@ -1878,7 +2233,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>105</v>
       </c>
@@ -1892,7 +2247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
@@ -1906,7 +2261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>78</v>
       </c>
@@ -1920,7 +2275,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>94</v>
       </c>
@@ -1937,7 +2292,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>104</v>
       </c>
@@ -1954,7 +2309,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -1971,7 +2326,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>104</v>
       </c>
@@ -1985,7 +2340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>104</v>
       </c>
@@ -1999,7 +2354,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2013,7 +2368,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -2030,7 +2385,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -2044,7 +2399,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -2058,7 +2413,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -2072,7 +2427,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -2100,7 +2455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -2114,7 +2469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -2128,7 +2483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>4</v>
       </c>
@@ -2142,7 +2497,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
@@ -2156,7 +2511,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -2184,7 +2539,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>4</v>
       </c>
@@ -2212,7 +2567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -2226,7 +2581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>4</v>
       </c>
@@ -2240,7 +2595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
@@ -2254,7 +2609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
@@ -2268,7 +2623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>4</v>
       </c>
@@ -2296,7 +2651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>4</v>
       </c>
@@ -2310,7 +2665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
@@ -2324,7 +2679,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>4</v>
       </c>
@@ -2338,7 +2693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>56</v>
       </c>
@@ -2355,7 +2710,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>56</v>
       </c>
@@ -2372,7 +2727,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>56</v>
       </c>
@@ -2386,7 +2741,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>56</v>
       </c>
@@ -2400,7 +2755,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>56</v>
       </c>
@@ -2414,7 +2769,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>65</v>
       </c>
@@ -2431,7 +2786,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>65</v>
       </c>
@@ -2448,7 +2803,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>65</v>
       </c>
@@ -2465,7 +2820,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>65</v>
       </c>
@@ -2479,7 +2834,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>65</v>
       </c>
@@ -2490,7 +2845,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>65</v>
       </c>
@@ -2498,7 +2853,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>65</v>
       </c>
@@ -2515,7 +2870,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>65</v>
       </c>
@@ -2523,7 +2878,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>65</v>
       </c>
@@ -2540,7 +2895,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>76</v>
       </c>
@@ -2557,7 +2912,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>76</v>
       </c>
@@ -2574,7 +2929,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>76</v>
       </c>
@@ -2591,7 +2946,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>76</v>
       </c>
@@ -2605,7 +2960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>76</v>
       </c>
@@ -2619,7 +2974,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>76</v>
       </c>
@@ -2633,7 +2988,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>76</v>
       </c>
@@ -2647,7 +3002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>76</v>
       </c>
@@ -2661,7 +3016,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>76</v>
       </c>
@@ -2675,7 +3030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>76</v>
       </c>
@@ -2689,7 +3044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
@@ -2718,14 +3073,988 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="6" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="E2" s="9">
+        <v>4.59</v>
+      </c>
+      <c r="F2" s="9">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9">
+        <v>25</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2.12</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2.12</v>
+      </c>
+      <c r="F3" s="9">
+        <v>29</v>
+      </c>
+      <c r="G3" s="9">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="E4" s="10">
+        <v>3.72</v>
+      </c>
+      <c r="F4" s="11">
+        <v>96</v>
+      </c>
+      <c r="G4" s="11">
+        <v>56</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="11">
+        <v>2.85</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2.67</v>
+      </c>
+      <c r="F6" s="11">
+        <v>68</v>
+      </c>
+      <c r="G6" s="11">
+        <v>79</v>
+      </c>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3.23</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2.52</v>
+      </c>
+      <c r="F8" s="11">
+        <v>30</v>
+      </c>
+      <c r="G8" s="11">
+        <v>29</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1.82</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1.81</v>
+      </c>
+      <c r="F10" s="9">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9">
+        <v>28</v>
+      </c>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="11">
+        <v>3.12</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="F11" s="11">
+        <v>45</v>
+      </c>
+      <c r="G11" s="11">
+        <v>35</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2.72</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3.28</v>
+      </c>
+      <c r="F13" s="11">
+        <v>25</v>
+      </c>
+      <c r="G13" s="11">
+        <v>26</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="11">
+        <v>3.08</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3.46</v>
+      </c>
+      <c r="F15" s="11">
+        <v>25</v>
+      </c>
+      <c r="G15" s="11">
+        <v>30</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2.88</v>
+      </c>
+      <c r="F17" s="11">
+        <v>31</v>
+      </c>
+      <c r="G17" s="11">
+        <v>28</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2.93</v>
+      </c>
+      <c r="E19" s="10">
+        <v>3.49</v>
+      </c>
+      <c r="F19" s="11">
+        <v>30</v>
+      </c>
+      <c r="G19" s="11">
+        <v>30</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1.27</v>
+      </c>
+      <c r="E21" s="9">
+        <v>3.38</v>
+      </c>
+      <c r="F21" s="9">
+        <v>28</v>
+      </c>
+      <c r="G21" s="9">
+        <v>28</v>
+      </c>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.93</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1.92</v>
+      </c>
+      <c r="F22" s="11">
+        <v>32</v>
+      </c>
+      <c r="G22" s="11">
+        <v>34</v>
+      </c>
+      <c r="H22" s="11">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2.16</v>
+      </c>
+      <c r="E26" s="15">
+        <v>2.82</v>
+      </c>
+      <c r="F26" s="11">
+        <v>30</v>
+      </c>
+      <c r="G26" s="11">
+        <v>36</v>
+      </c>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="11">
+        <v>3.94</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F28" s="11">
+        <v>70</v>
+      </c>
+      <c r="G28" s="11">
+        <v>92</v>
+      </c>
+      <c r="H28" s="11">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2.93</v>
+      </c>
+      <c r="E30" s="9">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="F30" s="9">
+        <v>34</v>
+      </c>
+      <c r="G30" s="9">
+        <v>32</v>
+      </c>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="11">
+        <v>3.82</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3.29</v>
+      </c>
+      <c r="F31" s="11">
+        <v>25</v>
+      </c>
+      <c r="G31" s="11">
+        <v>26</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="11">
+        <v>3.57</v>
+      </c>
+      <c r="E33" s="10">
+        <v>3.26</v>
+      </c>
+      <c r="F33" s="11">
+        <v>34</v>
+      </c>
+      <c r="G33" s="11">
+        <v>30</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="11">
+        <v>5.08</v>
+      </c>
+      <c r="E36" s="10">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="F36" s="11">
+        <v>105</v>
+      </c>
+      <c r="G36" s="11">
+        <v>132</v>
+      </c>
+      <c r="H36" s="11">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="11">
+        <v>2.31</v>
+      </c>
+      <c r="E38" s="10">
+        <v>2.16</v>
+      </c>
+      <c r="F38" s="11">
+        <v>59</v>
+      </c>
+      <c r="G38" s="11">
+        <v>99</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:8" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="9">
+        <v>2.66</v>
+      </c>
+      <c r="E40" s="9">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F40" s="9">
+        <v>33</v>
+      </c>
+      <c r="G40" s="9">
+        <v>32</v>
+      </c>
+      <c r="H40" s="11">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="F41" s="9">
+        <v>25</v>
+      </c>
+      <c r="G41" s="9">
+        <v>25</v>
+      </c>
+      <c r="H41" s="12"/>
+    </row>
+    <row r="42" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="E42" s="10">
+        <v>2.92</v>
+      </c>
+      <c r="F42" s="11">
+        <v>39</v>
+      </c>
+      <c r="G42" s="11">
+        <v>42</v>
+      </c>
+      <c r="H42" s="11">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="1:8" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="9">
+        <v>4.43</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9">
+        <v>36</v>
+      </c>
+      <c r="G44" s="9">
+        <v>45</v>
+      </c>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="9">
+        <v>2.99</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F45" s="9">
+        <v>39</v>
+      </c>
+      <c r="G45" s="9">
+        <v>45</v>
+      </c>
+      <c r="H45" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="109">
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2735,13 +4064,552 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="18">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D2" s="18">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="18">
+        <v>2.12</v>
+      </c>
+      <c r="D3" s="18">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="19">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2.85</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="19">
+        <v>3.23</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1.82</v>
+      </c>
+      <c r="D10" s="18">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="19">
+        <v>3.12</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="19">
+        <v>2.72</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="19">
+        <v>3.08</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="19">
+        <v>2.93</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1.27</v>
+      </c>
+      <c r="D21" s="18">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="19">
+        <v>1.93</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="19">
+        <v>2.16</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="19">
+        <v>3.94</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="18">
+        <v>2.93</v>
+      </c>
+      <c r="D28" s="18">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="19">
+        <v>3.82</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="19">
+        <v>3.57</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="19">
+        <v>5.08</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="19">
+        <v>2.31</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="18">
+        <v>2.66</v>
+      </c>
+      <c r="D38" s="18">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="19">
+        <v>2.25</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="18">
+        <v>4.43</v>
+      </c>
+      <c r="D42" s="18"/>
+    </row>
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
COMPLETED IMPACT FACTORS TABLE
</commit_message>
<xml_diff>
--- a/paper/Impact Factors.xlsx
+++ b/paper/Impact Factors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/Outliers/paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/addiew/Documents/GitHub/Outliers/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC517811-15FF-8F41-B8D6-17D37C83F8F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFECFF53-8433-6B48-B65D-C07F16F3C69E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1420" windowWidth="25600" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11080" yWindow="460" windowWidth="25600" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2012 and 2017 Impact Factors" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Clinical</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Psychological Science</t>
+  </si>
+  <si>
+    <t>APA</t>
+  </si>
+  <si>
+    <t>Wiley</t>
+  </si>
+  <si>
+    <t>Elsevier</t>
+  </si>
+  <si>
+    <t>Springer</t>
+  </si>
+  <si>
+    <t>Human Kinetics</t>
   </si>
 </sst>
 </file>
@@ -304,7 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -313,12 +328,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -335,6 +344,9 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -700,19 +712,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="15.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -722,17 +734,17 @@
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -742,13 +754,16 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6">
         <v>2.12</v>
       </c>
-      <c r="D2" s="8">
+      <c r="E2" s="6">
         <v>2.12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -759,13 +774,16 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="6">
         <v>4.8499999999999996</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="6">
         <v>4.59</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="7">
         <v>6.05</v>
       </c>
     </row>
@@ -776,13 +794,16 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="6">
         <v>4.2699999999999996</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="6">
         <v>3.72</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="7">
         <v>4.95</v>
       </c>
     </row>
@@ -793,13 +814,16 @@
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6">
         <v>2.85</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="6">
         <v>2.67</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="7">
         <v>2.96</v>
       </c>
     </row>
@@ -810,13 +834,16 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6">
         <v>3.23</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="6">
         <v>2.52</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="7">
         <v>4.09</v>
       </c>
     </row>
@@ -827,17 +854,17 @@
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6">
         <v>1.82</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="6">
         <v>1.81</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -847,13 +874,16 @@
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="6">
         <v>3.12</v>
       </c>
-      <c r="D8" s="8">
+      <c r="E8" s="6">
         <v>2.6</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="7">
         <v>3.32</v>
       </c>
     </row>
@@ -864,13 +894,16 @@
       <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6">
         <v>2.72</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="6">
         <v>3.28</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="7">
         <v>3.96</v>
       </c>
     </row>
@@ -881,13 +914,16 @@
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="6">
         <v>2.88</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="7">
         <v>4.08</v>
       </c>
     </row>
@@ -898,13 +934,16 @@
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="6">
         <v>3.08</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="6">
         <v>3.46</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="7">
         <v>5.24</v>
       </c>
     </row>
@@ -915,13 +954,16 @@
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6">
         <v>1.27</v>
       </c>
-      <c r="D12" s="8">
+      <c r="E12" s="6">
         <v>3.38</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -932,13 +974,16 @@
       <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6">
         <v>2.93</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="6">
         <v>3.49</v>
       </c>
-      <c r="E13" s="9">
+      <c r="F13" s="7">
         <v>4.46</v>
       </c>
     </row>
@@ -949,13 +994,16 @@
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="6">
         <v>2.16</v>
       </c>
-      <c r="D14" s="8">
+      <c r="E14" s="6">
         <v>2.82</v>
       </c>
-      <c r="E14" s="9">
+      <c r="F14" s="7">
         <v>2.92</v>
       </c>
     </row>
@@ -966,298 +1014,334 @@
       <c r="B15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="6">
         <v>1.93</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E15" s="6">
         <v>1.92</v>
       </c>
-      <c r="E15" s="9">
+      <c r="F15" s="7">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6">
         <v>3.94</v>
       </c>
-      <c r="D16" s="8">
+      <c r="E16" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E16" s="9">
+      <c r="F16" s="7">
         <v>3.96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="6">
         <v>2.93</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="6">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="6">
         <v>3.57</v>
       </c>
-      <c r="D18" s="8">
+      <c r="E18" s="6">
         <v>3.26</v>
       </c>
-      <c r="E18" s="9">
+      <c r="F18" s="7">
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="6">
         <v>3.82</v>
       </c>
-      <c r="D19" s="8">
+      <c r="E19" s="6">
         <v>3.29</v>
       </c>
-      <c r="E19" s="9">
+      <c r="F19" s="7">
         <v>3.73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="6">
         <v>2.99</v>
       </c>
-      <c r="D20" s="8">
+      <c r="E20" s="6">
         <v>3.31</v>
       </c>
-      <c r="E20" s="9">
+      <c r="F20" s="7">
         <v>3.92</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="6">
         <v>4.43</v>
       </c>
-      <c r="D21" s="8">
+      <c r="E21" s="6">
         <v>5.67</v>
       </c>
-      <c r="E21" s="9">
+      <c r="F21" s="7">
         <v>6.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="6">
         <v>2.25</v>
       </c>
-      <c r="D22" s="8">
+      <c r="E22" s="6">
         <v>2.92</v>
       </c>
-      <c r="E22" s="9">
+      <c r="F22" s="7">
         <v>3.49</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="6">
         <v>2.31</v>
       </c>
-      <c r="D23" s="8">
+      <c r="E23" s="6">
         <v>2.16</v>
       </c>
-      <c r="E23" s="9">
+      <c r="F23" s="7">
         <v>2.97</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="6">
         <v>5.08</v>
       </c>
-      <c r="D24" s="8">
+      <c r="E24" s="6">
         <v>5.0199999999999996</v>
       </c>
-      <c r="E24" s="9">
+      <c r="F24" s="7">
         <v>7.3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="6">
         <v>2.66</v>
       </c>
-      <c r="D25" s="8">
+      <c r="E25" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="8">
+      <c r="E26" s="6">
         <v>0.66</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="F26" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:L43">

</xml_diff>